<commit_message>
Revert "Merge pull request #50 from LindmanBassi/feature-20"
This reverts commit 76b016bc1e1a5fa9ae00869576947fe4877014d0, reversing
changes made to 05a9c2762def57d635f25545b3b40fb7b54a311f.
</commit_message>
<xml_diff>
--- a/6.Gerenciamento de Projeto/EvT - Checklist_Verificacao_de_Projeto.xlsx
+++ b/6.Gerenciamento de Projeto/EvT - Checklist_Verificacao_de_Projeto.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{9426F53B-BB86-402D-83F7-114097EA189B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8F329E4-5338-46AE-96E8-2FB6DB0377AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC7CC7D2-7AE8-4D24-A49B-1D8FF4C3575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="666" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -711,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="116">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1059,9 +1061,6 @@
   </si>
   <si>
     <t>Sim</t>
-  </si>
-  <si>
-    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -1484,10 +1483,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1538,6 +1533,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1645,7 +1646,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82608695652173914</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2608,10 +2609,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2620,22 +2621,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2831,7 +2832,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2855,13 +2856,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2950,22 +2951,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -7063,10 +7064,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7336,17 +7333,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:2" ht="18.5">
+      <c r="A1" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
@@ -7369,9 +7366,9 @@
       <c r="A4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="20" t="e">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.82608695652173914</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7412,16 +7409,16 @@
       <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="14" max="14" width="13.1796875" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -7479,21 +7476,21 @@
       <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P2" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q2" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>1</v>
-      </c>
-      <c r="R2" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R2" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7519,21 +7516,21 @@
       <c r="N3" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>1</v>
-      </c>
-      <c r="P3" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q3" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R3" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7559,21 +7556,21 @@
       <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0.75</v>
-      </c>
-      <c r="P4" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q4" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0.25</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7599,21 +7596,21 @@
       <c r="N5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q5" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R5" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7679,21 +7676,21 @@
       <c r="N7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0.75</v>
-      </c>
-      <c r="P7" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0.25</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7759,21 +7756,21 @@
       <c r="N9" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.6</v>
-      </c>
-      <c r="P9" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7799,21 +7796,21 @@
       <c r="N10" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="P10" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q10" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="R10" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R10" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7839,21 +7836,21 @@
       <c r="N11" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>1</v>
-      </c>
-      <c r="P11" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7879,21 +7876,21 @@
       <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="24" t="e">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0.5</v>
-      </c>
-      <c r="P12" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="24" t="e">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" s="24" t="e">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0.5</v>
-      </c>
-      <c r="R12" s="24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" s="24" t="e">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -8446,62 +8443,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B40" sqref="B40:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" style="4" customWidth="1"/>
     <col min="3" max="3" width="84" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.81640625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="4.453125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="6" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="45"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4">
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.5">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -8521,8 +8518,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.4">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:10" ht="14.5">
+      <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
@@ -8549,8 +8546,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.4">
-      <c r="A6" s="40"/>
+    <row r="6" spans="1:10" ht="14.5">
+      <c r="A6" s="38"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -8564,7 +8561,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9"/>
@@ -8592,7 +8589,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="36"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="30">
         <v>2</v>
       </c>
@@ -8605,8 +8602,8 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="14.4">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:10" ht="14.5">
+      <c r="A9" s="34"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -8619,8 +8616,8 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="14.4">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:10" ht="14.5">
+      <c r="A10" s="34"/>
       <c r="B10" s="5">
         <v>4</v>
       </c>
@@ -8633,8 +8630,8 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="14.4">
-      <c r="A11" s="36"/>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="14.5">
+      <c r="A11" s="34"/>
       <c r="B11" s="5">
         <v>5</v>
       </c>
@@ -8648,7 +8645,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A12" s="36"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="5">
         <v>6</v>
       </c>
@@ -8661,8 +8658,8 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="14.4">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:10" ht="14.5">
+      <c r="A13" s="34"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>3</v>
@@ -8687,8 +8684,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.8">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:10" ht="29">
+      <c r="A14" s="34"/>
       <c r="B14" s="29">
         <v>7</v>
       </c>
@@ -8701,8 +8698,8 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A15" s="36"/>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A15" s="34"/>
       <c r="B15" s="5">
         <v>8</v>
       </c>
@@ -8715,8 +8712,8 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A16" s="34"/>
       <c r="B16" s="5">
         <v>9</v>
       </c>
@@ -8729,8 +8726,8 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="14.4">
-      <c r="A17" s="36"/>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A17" s="34"/>
       <c r="B17" s="29">
         <v>10</v>
       </c>
@@ -8743,8 +8740,8 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="14.4">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="14.5">
+      <c r="A18" s="34"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -8757,8 +8754,8 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="14.4">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:10" ht="14.5">
+      <c r="A19" s="34"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
         <v>97</v>
@@ -8783,12 +8780,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8">
-      <c r="A20" s="36"/>
-      <c r="B20" s="5">
+    <row r="20" spans="1:10" ht="29">
+      <c r="A20" s="34"/>
+      <c r="B20" s="49">
         <v>12</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="48" t="s">
         <v>78</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -8797,12 +8794,12 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="28.8">
-      <c r="A21" s="36"/>
-      <c r="B21" s="5">
+    <row r="21" spans="1:10" ht="29">
+      <c r="A21" s="34"/>
+      <c r="B21" s="49">
         <v>13</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="48" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -8811,8 +8808,8 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="14.4">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:10" ht="14.5">
+      <c r="A22" s="34"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
         <v>4</v>
@@ -8837,12 +8834,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="28.8">
-      <c r="A23" s="36"/>
-      <c r="B23" s="5">
+    <row r="23" spans="1:10" ht="29">
+      <c r="A23" s="34"/>
+      <c r="B23" s="49">
         <v>14</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="48" t="s">
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -8851,8 +8848,8 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="14.4">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:10" ht="14.5">
+      <c r="A24" s="34"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -8865,8 +8862,8 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="14.4">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:10" ht="14.5">
+      <c r="A25" s="34"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
         <v>36</v>
@@ -8891,8 +8888,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.8">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:10" ht="29">
+      <c r="A26" s="34"/>
       <c r="B26" s="29">
         <v>16</v>
       </c>
@@ -8905,8 +8902,8 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="14.4">
-      <c r="A27" s="36"/>
+    <row r="27" spans="1:10" ht="14.5">
+      <c r="A27" s="34"/>
       <c r="B27" s="5">
         <v>17</v>
       </c>
@@ -8919,8 +8916,8 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="14.4">
-      <c r="A28" s="36"/>
+    <row r="28" spans="1:10" ht="14.5">
+      <c r="A28" s="34"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>13</v>
@@ -8945,12 +8942,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="28.8">
-      <c r="A29" s="36"/>
-      <c r="B29" s="5">
+    <row r="29" spans="1:10" ht="29">
+      <c r="A29" s="34"/>
+      <c r="B29" s="49">
         <v>21</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="48" t="s">
         <v>72</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -8959,8 +8956,8 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="14.4">
-      <c r="A30" s="36"/>
+    <row r="30" spans="1:10" ht="14.5">
+      <c r="A30" s="34"/>
       <c r="B30" s="5">
         <v>22</v>
       </c>
@@ -8973,8 +8970,8 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:10" ht="14.4">
-      <c r="A31" s="36"/>
+    <row r="31" spans="1:10" ht="14.5">
+      <c r="A31" s="34"/>
       <c r="B31" s="5">
         <v>23</v>
       </c>
@@ -8987,8 +8984,8 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="14.4">
-      <c r="A32" s="36"/>
+    <row r="32" spans="1:10" ht="14.5">
+      <c r="A32" s="34"/>
       <c r="B32" s="5">
         <v>24</v>
       </c>
@@ -9001,8 +8998,8 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="14.4">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:10" ht="14.5">
+      <c r="A33" s="34"/>
       <c r="B33" s="5">
         <v>25</v>
       </c>
@@ -9015,8 +9012,8 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4">
-      <c r="A34" s="36"/>
+    <row r="34" spans="1:10" ht="29">
+      <c r="A34" s="34"/>
       <c r="B34" s="5">
         <v>26</v>
       </c>
@@ -9028,8 +9025,8 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="14.4">
-      <c r="A35" s="36"/>
+    <row r="35" spans="1:10" ht="29">
+      <c r="A35" s="34"/>
       <c r="B35" s="5">
         <v>27</v>
       </c>
@@ -9042,8 +9039,8 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:10" ht="14.4">
-      <c r="A36" s="36"/>
+    <row r="36" spans="1:10" ht="14.5">
+      <c r="A36" s="34"/>
       <c r="B36" s="5">
         <v>28</v>
       </c>
@@ -9057,7 +9054,7 @@
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="9"/>
@@ -9084,8 +9081,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="28.8">
-      <c r="A38" s="35"/>
+    <row r="38" spans="1:10" ht="29">
+      <c r="A38" s="33"/>
       <c r="B38" s="29">
         <v>30</v>
       </c>
@@ -9098,12 +9095,12 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="14.4">
-      <c r="A39" s="35"/>
-      <c r="B39" s="5">
+    <row r="39" spans="1:10" ht="14.5">
+      <c r="A39" s="33"/>
+      <c r="B39" s="49">
         <v>31</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="48" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -9112,12 +9109,12 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4">
-      <c r="A40" s="35"/>
-      <c r="B40" s="5">
+    <row r="40" spans="1:10" ht="14.5">
+      <c r="A40" s="33"/>
+      <c r="B40" s="49">
         <v>32</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="48" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -9126,8 +9123,8 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="28.8">
-      <c r="A41" s="35"/>
+    <row r="41" spans="1:10" ht="29">
+      <c r="A41" s="33"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -9167,59 +9164,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" style="4" customWidth="1"/>
     <col min="3" max="3" width="68" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.7265625" customWidth="1"/>
     <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="21">
+      <c r="E2" s="43"/>
+      <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.82608695652173914</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4">
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.5">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -9240,7 +9237,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9251,17 +9248,15 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="14.4">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:10" ht="14.5">
+      <c r="A6" s="34"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
@@ -9274,15 +9269,15 @@
       </c>
       <c r="I6">
         <f>COUNTIF(D6,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>COUNTIF(D6,"NA")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:10" ht="14.5">
+      <c r="A7" s="34"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -9291,22 +9286,20 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A8" s="36"/>
-      <c r="B8" s="29">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A8" s="34"/>
+      <c r="B8" s="5">
         <v>2</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -9321,26 +9314,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A9" s="34"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="32"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10" ht="14.4">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:10" ht="14.5">
+      <c r="A10" s="34"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
         <v>97</v>
@@ -9349,22 +9340,20 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="28.8">
-      <c r="A11" s="36"/>
-      <c r="B11" s="29">
+    <row r="11" spans="1:10" ht="29">
+      <c r="A11" s="34"/>
+      <c r="B11" s="22">
         <v>4</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11">
         <f>COUNTIF(D11:D14,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <f>COUNTIF(D11:D14,"Parcialmente")</f>
@@ -9376,53 +9365,47 @@
       </c>
       <c r="J11">
         <f>COUNTIF(D11:D14,"NA")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.8">
-      <c r="A12" s="36"/>
-      <c r="B12" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29">
+      <c r="A12" s="34"/>
+      <c r="B12" s="22">
         <v>5</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="14.4">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:10" ht="14.5">
+      <c r="A13" s="34"/>
       <c r="B13" s="5">
         <v>6</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:10" ht="29">
+      <c r="A14" s="34"/>
       <c r="B14" s="5">
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="14.4">
-      <c r="A15" s="36"/>
+    <row r="15" spans="1:10" ht="14.5">
+      <c r="A15" s="34"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>4</v>
@@ -9431,17 +9414,15 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="14.4">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:10" ht="14.5">
+      <c r="A16" s="34"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
@@ -9458,11 +9439,11 @@
       </c>
       <c r="J16">
         <f>COUNTIF(D16,"NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="9"/>
@@ -9473,22 +9454,20 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="28.8">
-      <c r="A18" s="36"/>
-      <c r="B18" s="29">
+    <row r="18" spans="1:10" ht="29">
+      <c r="A18" s="34"/>
+      <c r="B18" s="5">
         <v>9</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
@@ -9500,53 +9479,47 @@
       </c>
       <c r="J18">
         <f>COUNTIF(D18:D21,"NA")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.8">
-      <c r="A19" s="36"/>
-      <c r="B19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="29">
+      <c r="A19" s="34"/>
+      <c r="B19" s="22">
         <v>10</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>115</v>
-      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A20" s="34"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="28.8">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:10" ht="29">
+      <c r="A21" s="34"/>
       <c r="B21" s="5">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="14.4">
-      <c r="A22" s="39" t="s">
+    <row r="22" spans="1:10" ht="14.5">
+      <c r="A22" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="9"/>
@@ -9557,22 +9530,20 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:10" ht="28.8">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:10" ht="29">
+      <c r="A23" s="34"/>
       <c r="B23" s="5">
         <v>17</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
@@ -9584,67 +9555,59 @@
       </c>
       <c r="J23">
         <f>COUNTIF(D23:D27,"NA")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28.8">
-      <c r="A24" s="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="29">
+      <c r="A24" s="34"/>
       <c r="B24" s="5">
         <v>18</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="28.8">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:10" ht="29">
+      <c r="A25" s="34"/>
       <c r="B25" s="5">
         <v>19</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="14.4">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:10" ht="14.5">
+      <c r="A26" s="34"/>
       <c r="B26" s="5">
         <v>21</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="14.4">
-      <c r="A27" s="36"/>
+    <row r="27" spans="1:10" ht="14.5">
+      <c r="A27" s="34"/>
       <c r="B27" s="5">
         <v>22</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="14.4">
-      <c r="A28" s="46" t="s">
+    <row r="28" spans="1:10" ht="14.5">
+      <c r="A28" s="44" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="9"/>
@@ -9655,22 +9618,20 @@
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:10" ht="14.4">
-      <c r="A29" s="46"/>
+    <row r="29" spans="1:10" ht="14.5">
+      <c r="A29" s="44"/>
       <c r="B29" s="5">
         <v>23</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
@@ -9678,85 +9639,75 @@
       </c>
       <c r="I29">
         <f>COUNTIF(D29:D34,"Não")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <f>COUNTIF(D29:D34,"NA")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4">
-      <c r="A30" s="46"/>
+    <row r="30" spans="1:10" ht="14.5">
+      <c r="A30" s="44"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:10" ht="28.8">
-      <c r="A31" s="46"/>
+    <row r="31" spans="1:10" ht="29">
+      <c r="A31" s="44"/>
       <c r="B31" s="5">
         <v>25</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="14.4">
-      <c r="A32" s="46"/>
+    <row r="32" spans="1:10" ht="14.5">
+      <c r="A32" s="44"/>
       <c r="B32" s="5">
         <v>26</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="14.4">
-      <c r="A33" s="46"/>
+    <row r="33" spans="1:10" ht="14.5">
+      <c r="A33" s="44"/>
       <c r="B33" s="5">
         <v>27</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4">
-      <c r="A34" s="46"/>
+    <row r="34" spans="1:10" ht="14.5">
+      <c r="A34" s="44"/>
       <c r="B34" s="5">
         <v>28</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -9767,22 +9718,20 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:10" ht="28.8">
-      <c r="A36" s="35"/>
+    <row r="36" spans="1:10" ht="29">
+      <c r="A36" s="33"/>
       <c r="B36" s="5">
         <v>29</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
@@ -9797,36 +9746,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:10" ht="14.5">
+      <c r="A37" s="33"/>
       <c r="B37" s="5">
         <v>30</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="28.8">
-      <c r="A38" s="35"/>
+    <row r="38" spans="1:10" ht="29">
+      <c r="A38" s="33"/>
       <c r="B38" s="5">
         <v>31</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D38" s="3"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="14.4">
-      <c r="A39" s="35"/>
+    <row r="39" spans="1:10" ht="14.5">
+      <c r="A39" s="33"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
         <v>15</v>
@@ -9835,22 +9780,20 @@
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4">
-      <c r="A40" s="35"/>
+    <row r="40" spans="1:10" ht="14.5">
+      <c r="A40" s="33"/>
       <c r="B40" s="5">
         <v>32</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40">
         <f>COUNTIF(D40:D41,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <f>COUNTIF(D40:D41,"Parcialmente")</f>
@@ -9858,24 +9801,22 @@
       </c>
       <c r="I40">
         <f>COUNTIF(D40:D41,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <f>COUNTIF(D40:D41,"NA")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4">
-      <c r="A41" s="35"/>
+    <row r="41" spans="1:10" ht="14.5">
+      <c r="A41" s="33"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -9913,55 +9854,55 @@
       <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="10" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="71.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.7265625" customWidth="1"/>
+    <col min="7" max="10" width="9.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="45"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4">
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.5">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -9982,7 +9923,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9993,8 +9934,8 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="14.4">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:10" ht="14.5">
+      <c r="A6" s="34"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -10021,8 +9962,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:10" ht="14.5">
+      <c r="A7" s="34"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -10031,8 +9972,8 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A8" s="36"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A8" s="34"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -10059,8 +10000,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:10" ht="14.5">
+      <c r="A9" s="34"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>97</v>
@@ -10069,8 +10010,8 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:10" ht="29">
+      <c r="A10" s="34"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10097,8 +10038,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8">
-      <c r="A11" s="36"/>
+    <row r="11" spans="1:10" ht="29">
+      <c r="A11" s="34"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10110,7 +10051,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A12" s="36"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10121,8 +10062,8 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="14.4">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:10" ht="14.5">
+      <c r="A13" s="34"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10131,8 +10072,8 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="14.4">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:10" ht="14.5">
+      <c r="A14" s="34"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10160,7 +10101,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10171,8 +10112,8 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="14.4">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:10" ht="14.5">
+      <c r="A16" s="34"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10199,8 +10140,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4">
-      <c r="A17" s="39" t="s">
+    <row r="17" spans="1:10" ht="14.5">
+      <c r="A17" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10211,8 +10152,8 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="14.4">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:10" ht="14.5">
+      <c r="A18" s="34"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -10239,8 +10180,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28.8">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:10" ht="29">
+      <c r="A19" s="34"/>
       <c r="B19" s="5">
         <v>13</v>
       </c>
@@ -10251,8 +10192,8 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="28.8">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:10" ht="29">
+      <c r="A20" s="34"/>
       <c r="B20" s="5">
         <v>14</v>
       </c>
@@ -10263,8 +10204,8 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="14.4">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:10" ht="14.5">
+      <c r="A21" s="34"/>
       <c r="B21" s="5">
         <v>15</v>
       </c>
@@ -10275,8 +10216,8 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="14.4">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:10" ht="14.5">
+      <c r="A22" s="34"/>
       <c r="B22" s="5">
         <v>16</v>
       </c>
@@ -10287,8 +10228,8 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="14.4">
-      <c r="A23" s="39" t="s">
+    <row r="23" spans="1:10" ht="14.5">
+      <c r="A23" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="9"/>
@@ -10299,8 +10240,8 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:10" ht="28.8">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:10" ht="29">
+      <c r="A24" s="34"/>
       <c r="B24" s="22">
         <v>17</v>
       </c>
@@ -10327,8 +10268,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.8">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:10" ht="29">
+      <c r="A25" s="34"/>
       <c r="B25" s="5">
         <v>18</v>
       </c>
@@ -10339,8 +10280,8 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="14.4">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:10" ht="14.5">
+      <c r="A26" s="34"/>
       <c r="B26" s="5">
         <v>19</v>
       </c>
@@ -10351,8 +10292,8 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="14.4">
-      <c r="A27" s="36"/>
+    <row r="27" spans="1:10" ht="14.5">
+      <c r="A27" s="34"/>
       <c r="B27" s="5">
         <v>21</v>
       </c>
@@ -10363,8 +10304,8 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="14.4">
-      <c r="A28" s="36"/>
+    <row r="28" spans="1:10" ht="14.5">
+      <c r="A28" s="34"/>
       <c r="B28" s="5">
         <v>22</v>
       </c>
@@ -10375,8 +10316,8 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:10" ht="14.4">
-      <c r="A29" s="46" t="s">
+    <row r="29" spans="1:10" ht="14.5">
+      <c r="A29" s="44" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="9"/>
@@ -10387,8 +10328,8 @@
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:10" ht="14.4">
-      <c r="A30" s="46"/>
+    <row r="30" spans="1:10" ht="14.5">
+      <c r="A30" s="44"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -10415,8 +10356,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.8">
-      <c r="A31" s="46"/>
+    <row r="31" spans="1:10" ht="29">
+      <c r="A31" s="44"/>
       <c r="B31" s="5">
         <v>26</v>
       </c>
@@ -10427,8 +10368,8 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="14.4">
-      <c r="A32" s="46"/>
+    <row r="32" spans="1:10" ht="14.5">
+      <c r="A32" s="44"/>
       <c r="B32" s="5">
         <v>27</v>
       </c>
@@ -10439,8 +10380,8 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="14.4">
-      <c r="A33" s="46"/>
+    <row r="33" spans="1:10" ht="14.5">
+      <c r="A33" s="44"/>
       <c r="B33" s="5">
         <v>28</v>
       </c>
@@ -10451,8 +10392,8 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4">
-      <c r="A34" s="46"/>
+    <row r="34" spans="1:10" ht="14.5">
+      <c r="A34" s="44"/>
       <c r="B34" s="5">
         <v>29</v>
       </c>
@@ -10464,7 +10405,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -10475,8 +10416,8 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="1:10" ht="28.8">
-      <c r="A36" s="35"/>
+    <row r="36" spans="1:10" ht="29">
+      <c r="A36" s="33"/>
       <c r="B36" s="5">
         <v>30</v>
       </c>
@@ -10503,8 +10444,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:10" ht="14.5">
+      <c r="A37" s="33"/>
       <c r="B37" s="5">
         <v>31</v>
       </c>
@@ -10515,8 +10456,8 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="28.8">
-      <c r="A38" s="35"/>
+    <row r="38" spans="1:10" ht="29">
+      <c r="A38" s="33"/>
       <c r="B38" s="5">
         <v>32</v>
       </c>
@@ -10527,8 +10468,8 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="14.4">
-      <c r="A39" s="35"/>
+    <row r="39" spans="1:10" ht="14.5">
+      <c r="A39" s="33"/>
       <c r="B39" s="5"/>
       <c r="C39" s="8" t="s">
         <v>105</v>
@@ -10537,8 +10478,8 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4">
-      <c r="A40" s="35"/>
+    <row r="40" spans="1:10" ht="14.5">
+      <c r="A40" s="33"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
         <v>15</v>
@@ -10547,8 +10488,8 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:10" ht="14.4">
-      <c r="A41" s="35"/>
+    <row r="41" spans="1:10" ht="14.5">
+      <c r="A41" s="33"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -10575,8 +10516,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.4">
-      <c r="A42" s="35"/>
+    <row r="42" spans="1:10" ht="14.5">
+      <c r="A42" s="33"/>
       <c r="B42" s="5">
         <v>34</v>
       </c>
@@ -10587,31 +10528,31 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="51" spans="2:3" ht="14.4">
+    <row r="51" spans="2:3" ht="14.5">
       <c r="B51"/>
       <c r="C51"/>
     </row>
-    <row r="52" spans="2:3" ht="14.4">
+    <row r="52" spans="2:3" ht="14.5">
       <c r="B52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="2:3" ht="14.4">
+    <row r="53" spans="2:3" ht="14.5">
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="2:3" ht="14.4">
+    <row r="54" spans="2:3" ht="14.5">
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="2:3" ht="14.4">
+    <row r="55" spans="2:3" ht="14.5">
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="2:3" ht="14.4">
+    <row r="56" spans="2:3" ht="14.5">
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="2:3" ht="14.4">
+    <row r="57" spans="2:3" ht="14.5">
       <c r="B57"/>
       <c r="C57"/>
     </row>
@@ -10650,55 +10591,55 @@
       <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="71.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.7265625" customWidth="1"/>
     <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="45"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D43,"Sim")/(COUNTA(D5:D43)-COUNTIF(D5:D43,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4">
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.5">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -10719,7 +10660,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -10730,8 +10671,8 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="14.4">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:10" ht="14.5">
+      <c r="A6" s="34"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -10758,8 +10699,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:10" ht="14.5">
+      <c r="A7" s="34"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -10768,8 +10709,8 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A8" s="36"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A8" s="34"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -10796,8 +10737,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:10" ht="14.5">
+      <c r="A9" s="34"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>14</v>
@@ -10806,8 +10747,8 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8">
-      <c r="A10" s="36"/>
+    <row r="10" spans="1:10" ht="29">
+      <c r="A10" s="34"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10834,8 +10775,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8">
-      <c r="A11" s="36"/>
+    <row r="11" spans="1:10" ht="29">
+      <c r="A11" s="34"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10847,7 +10788,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A12" s="36"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10858,8 +10799,8 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="14.4">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:10" ht="14.5">
+      <c r="A13" s="34"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10868,8 +10809,8 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="14.4">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:10" ht="14.5">
+      <c r="A14" s="34"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10897,7 +10838,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10908,8 +10849,8 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="14.4">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:10" ht="14.5">
+      <c r="A16" s="34"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10937,7 +10878,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10948,8 +10889,8 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:10" ht="14.4">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:10" ht="14.5">
+      <c r="A18" s="34"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -10976,8 +10917,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.4">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:10" ht="14.5">
+      <c r="A19" s="34"/>
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -10988,8 +10929,8 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="28.8">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:10" ht="29">
+      <c r="A20" s="34"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -11000,8 +10941,8 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="14.4">
-      <c r="A21" s="40"/>
+    <row r="21" spans="1:10" ht="14.5">
+      <c r="A21" s="38"/>
       <c r="B21" s="5">
         <v>13</v>
       </c>
@@ -11012,8 +10953,8 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="14.4">
-      <c r="A22" s="39" t="s">
+    <row r="22" spans="1:10" ht="14.5">
+      <c r="A22" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="9"/>
@@ -11024,8 +10965,8 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:10" ht="14.4">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:10" ht="14.5">
+      <c r="A23" s="34"/>
       <c r="B23" s="5">
         <v>14</v>
       </c>
@@ -11052,8 +10993,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.4">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:10" ht="14.5">
+      <c r="A24" s="34"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -11065,7 +11006,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="9"/>
@@ -11076,8 +11017,8 @@
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="28.8">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="29">
+      <c r="A26" s="34"/>
       <c r="B26" s="22">
         <v>24</v>
       </c>
@@ -11104,8 +11045,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="43.2">
-      <c r="A27" s="36"/>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="43.5">
+      <c r="A27" s="34"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -11116,8 +11057,8 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="14.4">
-      <c r="A28" s="36"/>
+    <row r="28" spans="1:10" ht="14.5">
+      <c r="A28" s="34"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>10</v>
@@ -11126,8 +11067,8 @@
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:10" ht="28.8">
-      <c r="A29" s="36"/>
+    <row r="29" spans="1:10" ht="29">
+      <c r="A29" s="34"/>
       <c r="B29" s="22">
         <v>26</v>
       </c>
@@ -11154,8 +11095,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4">
-      <c r="A30" s="46" t="s">
+    <row r="30" spans="1:10" ht="14.5">
+      <c r="A30" s="44" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="9"/>
@@ -11166,8 +11107,8 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:10" ht="14.4">
-      <c r="A31" s="46"/>
+    <row r="31" spans="1:10" ht="14.5">
+      <c r="A31" s="44"/>
       <c r="B31" s="5">
         <v>19</v>
       </c>
@@ -11194,8 +11135,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="28.8">
-      <c r="A32" s="46"/>
+    <row r="32" spans="1:10" ht="29">
+      <c r="A32" s="44"/>
       <c r="B32" s="5">
         <v>20</v>
       </c>
@@ -11206,8 +11147,8 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="14.4">
-      <c r="A33" s="46"/>
+    <row r="33" spans="1:10" ht="14.5">
+      <c r="A33" s="44"/>
       <c r="B33" s="5">
         <v>21</v>
       </c>
@@ -11218,8 +11159,8 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4">
-      <c r="A34" s="46"/>
+    <row r="34" spans="1:10" ht="14.5">
+      <c r="A34" s="44"/>
       <c r="B34" s="5">
         <v>24</v>
       </c>
@@ -11230,8 +11171,8 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="14.4">
-      <c r="A35" s="46"/>
+    <row r="35" spans="1:10" ht="14.5">
+      <c r="A35" s="44"/>
       <c r="B35" s="5">
         <v>25</v>
       </c>
@@ -11243,7 +11184,7 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="9"/>
@@ -11254,8 +11195,8 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:10" ht="28.8">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:10" ht="29">
+      <c r="A37" s="33"/>
       <c r="B37" s="5">
         <v>26</v>
       </c>
@@ -11282,8 +11223,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.4">
-      <c r="A38" s="35"/>
+    <row r="38" spans="1:10" ht="14.5">
+      <c r="A38" s="33"/>
       <c r="B38" s="5">
         <v>27</v>
       </c>
@@ -11294,8 +11235,8 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="28.8">
-      <c r="A39" s="35"/>
+    <row r="39" spans="1:10" ht="29">
+      <c r="A39" s="33"/>
       <c r="B39" s="5">
         <v>28</v>
       </c>
@@ -11306,8 +11247,8 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4">
-      <c r="A40" s="35"/>
+    <row r="40" spans="1:10" ht="14.5">
+      <c r="A40" s="33"/>
       <c r="B40" s="5"/>
       <c r="C40" s="8" t="s">
         <v>105</v>
@@ -11316,8 +11257,8 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="14.4">
-      <c r="A41" s="35"/>
+    <row r="41" spans="1:10" ht="14.5">
+      <c r="A41" s="33"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
         <v>15</v>
@@ -11326,8 +11267,8 @@
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:10" ht="14.4">
-      <c r="A42" s="35"/>
+    <row r="42" spans="1:10" ht="14.5">
+      <c r="A42" s="33"/>
       <c r="B42" s="5">
         <v>29</v>
       </c>
@@ -11354,8 +11295,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.4">
-      <c r="A43" s="35"/>
+    <row r="43" spans="1:10" ht="14.5">
+      <c r="A43" s="33"/>
       <c r="B43" s="5">
         <v>30</v>
       </c>
@@ -11366,31 +11307,31 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="52" spans="2:3" ht="14.4">
+    <row r="52" spans="2:3" ht="14.5">
       <c r="B52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="2:3" ht="14.4">
+    <row r="53" spans="2:3" ht="14.5">
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="2:3" ht="14.4">
+    <row r="54" spans="2:3" ht="14.5">
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="2:3" ht="14.4">
+    <row r="55" spans="2:3" ht="14.5">
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="2:3" ht="14.4">
+    <row r="56" spans="2:3" ht="14.5">
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="2:3" ht="14.4">
+    <row r="57" spans="2:3" ht="14.5">
       <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="2:3" ht="14.4">
+    <row r="58" spans="2:3" ht="14.5">
       <c r="B58"/>
       <c r="C58"/>
     </row>

</xml_diff>